<commit_message>
FixedCrops and sum at founds
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>Nome</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Preço Especial</t>
+  </si>
+  <si>
+    <t>Fixo</t>
   </si>
   <si>
     <t>Chivíria</t>
@@ -364,10 +367,13 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>20.0</v>
@@ -379,10 +385,10 @@
         <v>35.0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1">
         <v>0.0</v>
@@ -390,10 +396,13 @@
       <c r="H2" s="1">
         <v>25.0</v>
       </c>
+      <c r="K2" s="1">
+        <v>10.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>50.0</v>
@@ -405,10 +414,10 @@
         <v>80.0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1">
         <v>0.0</v>
@@ -416,10 +425,13 @@
       <c r="H3" s="1">
         <v>62.0</v>
       </c>
+      <c r="K3" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>60.0</v>
@@ -431,10 +443,10 @@
         <v>40.0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="1">
         <v>3.0</v>
@@ -442,10 +454,13 @@
       <c r="H4" s="1">
         <v>75.0</v>
       </c>
+      <c r="K4" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1">
         <v>70.0</v>
@@ -457,10 +472,10 @@
         <v>110.0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G5" s="1">
         <v>0.0</v>
@@ -468,10 +483,13 @@
       <c r="H5" s="1">
         <v>87.0</v>
       </c>
+      <c r="K5" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
         <v>80.0</v>
@@ -483,10 +501,10 @@
         <v>175.0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G6" s="1">
         <v>0.0</v>
@@ -494,10 +512,13 @@
       <c r="H6" s="1">
         <v>100.0</v>
       </c>
+      <c r="K6" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1">
         <v>8.0</v>
@@ -506,10 +527,10 @@
         <v>120.0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G7" s="1">
         <v>4.0</v>
@@ -520,10 +541,13 @@
       <c r="J7" s="1">
         <v>100.0</v>
       </c>
+      <c r="K7" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1">
         <v>30.0</v>
@@ -535,10 +559,10 @@
         <v>50.0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G8" s="1">
         <v>0.0</v>
@@ -546,10 +570,13 @@
       <c r="H8" s="1">
         <v>37.0</v>
       </c>
+      <c r="K8" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1">
         <v>20.0</v>
@@ -561,16 +588,19 @@
         <v>30.0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G9" s="1">
         <v>0.0</v>
       </c>
       <c r="H9" s="1">
         <v>25.0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>